<commit_message>
Fixed all Arelle errors
</commit_message>
<xml_diff>
--- a/input_files/acfrs/Clayton_acfr_simple.xlsx
+++ b/input_files/acfrs/Clayton_acfr_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C09D8-35DD-1E4D-B632-E96398316613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAA4EE9-2B32-D64F-98C7-81DA7A3602DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1080" windowWidth="25200" windowHeight="14360" tabRatio="834" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="295">
   <si>
     <t>City of Clayton</t>
   </si>
@@ -2215,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3156,10 +3156,18 @@
       <c r="E39" s="8">
         <v>187452</v>
       </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="F39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="8">
+        <v>681698</v>
+      </c>
+      <c r="H39" s="8">
+        <v>-850946</v>
+      </c>
+      <c r="I39" s="8">
+        <v>-179685</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
@@ -3169,18 +3177,6 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="8">
-        <v>681698</v>
-      </c>
-      <c r="H40" s="8">
-        <v>-850946</v>
-      </c>
-      <c r="I40" s="8">
-        <v>-179685</v>
-      </c>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
@@ -3265,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3615,9 +3611,7 @@
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -3630,9 +3624,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
@@ -3645,9 +3637,7 @@
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
@@ -3845,9 +3835,7 @@
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -3929,9 +3917,7 @@
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F32" s="6"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
@@ -3953,7 +3939,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>14</v>
@@ -4436,7 +4422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4759,8 +4745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding support for dependency downloads for Arelle and ixbrl viewer
</commit_message>
<xml_diff>
--- a/input_files/acfrs/Clayton_acfr_simple.xlsx
+++ b/input_files/acfrs/Clayton_acfr_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAA4EE9-2B32-D64F-98C7-81DA7A3602DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB49FD-9C83-D946-81C6-7FFE86DEAD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -1417,13 +1417,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="44.5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
     <col min="3" max="5" width="18.6640625" customWidth="1"/>
   </cols>
@@ -2215,7 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -4745,7 +4745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>

</xml_diff>